<commit_message>
Restructured notebook. Working good
</commit_message>
<xml_diff>
--- a/DriverDrowsiness/results/output_eye.xlsx
+++ b/DriverDrowsiness/results/output_eye.xlsx
@@ -571,16 +571,16 @@
         <v>16</v>
       </c>
       <c r="L2" t="n">
-        <v>85.00000238418579</v>
+        <v>64.99999761581421</v>
       </c>
       <c r="M2" t="n">
         <v>3.196109771728516</v>
       </c>
       <c r="N2" t="n">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="O2" t="n">
-        <v>0.66</v>
+        <v>0.22</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
@@ -644,16 +644,16 @@
         <v>32</v>
       </c>
       <c r="L3" t="n">
-        <v>80.0000011920929</v>
+        <v>85.00000238418579</v>
       </c>
       <c r="M3" t="n">
         <v>3.196109771728516</v>
       </c>
       <c r="N3" t="n">
-        <v>1</v>
+        <v>0.92</v>
       </c>
       <c r="O3" t="n">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
@@ -717,16 +717,16 @@
         <v>64</v>
       </c>
       <c r="L4" t="n">
-        <v>68.00000071525574</v>
+        <v>76.99999809265137</v>
       </c>
       <c r="M4" t="n">
         <v>3.196109771728516</v>
       </c>
       <c r="N4" t="n">
-        <v>1</v>
+        <v>0.88</v>
       </c>
       <c r="O4" t="n">
-        <v>0.16</v>
+        <v>0.68</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
@@ -790,7 +790,7 @@
         <v>16</v>
       </c>
       <c r="L5" t="n">
-        <v>75.99999904632568</v>
+        <v>81.00000023841858</v>
       </c>
       <c r="M5" t="n">
         <v>3.196109771728516</v>
@@ -799,7 +799,7 @@
         <v>1</v>
       </c>
       <c r="O5" t="n">
-        <v>0.38</v>
+        <v>0.5</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
@@ -863,7 +863,7 @@
         <v>32</v>
       </c>
       <c r="L6" t="n">
-        <v>86.00000143051147</v>
+        <v>68.00000071525574</v>
       </c>
       <c r="M6" t="n">
         <v>3.196109771728516</v>
@@ -872,7 +872,7 @@
         <v>1</v>
       </c>
       <c r="O6" t="n">
-        <v>0.62</v>
+        <v>0.26</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
@@ -936,16 +936,16 @@
         <v>64</v>
       </c>
       <c r="L7" t="n">
-        <v>68.99999976158142</v>
+        <v>57.99999833106995</v>
       </c>
       <c r="M7" t="n">
         <v>3.196109771728516</v>
       </c>
       <c r="N7" t="n">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="O7" t="n">
-        <v>0.36</v>
+        <v>0.1</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
@@ -1009,16 +1009,16 @@
         <v>16</v>
       </c>
       <c r="L8" t="n">
-        <v>86.00000143051147</v>
+        <v>69.9999988079071</v>
       </c>
       <c r="M8" t="n">
         <v>1.617740631103516</v>
       </c>
       <c r="N8" t="n">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="O8" t="n">
-        <v>0.66</v>
+        <v>0.4</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
@@ -1082,16 +1082,16 @@
         <v>32</v>
       </c>
       <c r="L9" t="n">
-        <v>50</v>
+        <v>69.9999988079071</v>
       </c>
       <c r="M9" t="n">
         <v>1.617740631103516</v>
       </c>
       <c r="N9" t="n">
-        <v>1</v>
+        <v>0.92</v>
       </c>
       <c r="O9" t="n">
-        <v>0</v>
+        <v>0.26</v>
       </c>
       <c r="P9" t="inlineStr">
         <is>
@@ -1155,7 +1155,7 @@
         <v>64</v>
       </c>
       <c r="L10" t="n">
-        <v>51.99999809265137</v>
+        <v>50.99999904632568</v>
       </c>
       <c r="M10" t="n">
         <v>1.617740631103516</v>
@@ -1164,7 +1164,7 @@
         <v>1</v>
       </c>
       <c r="O10" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
         <v>16</v>
       </c>
       <c r="L11" t="n">
-        <v>76.99999809265137</v>
+        <v>56.00000023841858</v>
       </c>
       <c r="M11" t="n">
         <v>1.617740631103516</v>
@@ -1237,7 +1237,7 @@
         <v>1</v>
       </c>
       <c r="O11" t="n">
-        <v>0.48</v>
+        <v>0.08</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
@@ -1301,7 +1301,7 @@
         <v>32</v>
       </c>
       <c r="L12" t="n">
-        <v>70.99999785423279</v>
+        <v>56.00000023841858</v>
       </c>
       <c r="M12" t="n">
         <v>1.617740631103516</v>
@@ -1310,7 +1310,7 @@
         <v>1</v>
       </c>
       <c r="O12" t="n">
-        <v>0.22</v>
+        <v>0.1</v>
       </c>
       <c r="P12" t="inlineStr">
         <is>
@@ -1374,7 +1374,7 @@
         <v>64</v>
       </c>
       <c r="L13" t="n">
-        <v>51.99999809265137</v>
+        <v>52.99999713897705</v>
       </c>
       <c r="M13" t="n">
         <v>1.617740631103516</v>
@@ -1383,7 +1383,7 @@
         <v>1</v>
       </c>
       <c r="O13" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="P13" t="inlineStr">
         <is>
@@ -1447,16 +1447,16 @@
         <v>16</v>
       </c>
       <c r="L14" t="n">
-        <v>87.00000047683716</v>
+        <v>77.99999713897705</v>
       </c>
       <c r="M14" t="n">
         <v>3.177555084228516</v>
       </c>
       <c r="N14" t="n">
-        <v>0.84</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="O14" t="n">
-        <v>0.84</v>
+        <v>0.58</v>
       </c>
       <c r="P14" t="inlineStr">
         <is>
@@ -1520,16 +1520,16 @@
         <v>32</v>
       </c>
       <c r="L15" t="n">
-        <v>87.99999952316284</v>
+        <v>92.00000166893005</v>
       </c>
       <c r="M15" t="n">
         <v>3.177555084228516</v>
       </c>
       <c r="N15" t="n">
-        <v>0.9</v>
+        <v>0.88</v>
       </c>
       <c r="O15" t="n">
-        <v>0.84</v>
+        <v>1</v>
       </c>
       <c r="P15" t="inlineStr">
         <is>
@@ -1593,7 +1593,7 @@
         <v>64</v>
       </c>
       <c r="L16" t="n">
-        <v>51.99999809265137</v>
+        <v>56.00000023841858</v>
       </c>
       <c r="M16" t="n">
         <v>3.177555084228516</v>
@@ -1666,16 +1666,16 @@
         <v>16</v>
       </c>
       <c r="L17" t="n">
-        <v>72.00000286102295</v>
+        <v>88.99999856948853</v>
       </c>
       <c r="M17" t="n">
         <v>3.177555084228516</v>
       </c>
       <c r="N17" t="n">
-        <v>1</v>
+        <v>0.86</v>
       </c>
       <c r="O17" t="n">
-        <v>0.4</v>
+        <v>0.84</v>
       </c>
       <c r="P17" t="inlineStr">
         <is>
@@ -1739,16 +1739,16 @@
         <v>32</v>
       </c>
       <c r="L18" t="n">
-        <v>89.99999761581421</v>
+        <v>88.99999856948853</v>
       </c>
       <c r="M18" t="n">
         <v>3.177555084228516</v>
       </c>
       <c r="N18" t="n">
-        <v>0.8</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="O18" t="n">
-        <v>0.96</v>
+        <v>0.78</v>
       </c>
       <c r="P18" t="inlineStr">
         <is>
@@ -1812,7 +1812,7 @@
         <v>64</v>
       </c>
       <c r="L19" t="n">
-        <v>51.99999809265137</v>
+        <v>56.99999928474426</v>
       </c>
       <c r="M19" t="n">
         <v>3.177555084228516</v>
@@ -1821,7 +1821,7 @@
         <v>1</v>
       </c>
       <c r="O19" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="P19" t="inlineStr">
         <is>
@@ -1885,7 +1885,7 @@
         <v>16</v>
       </c>
       <c r="L20" t="n">
-        <v>54.00000214576721</v>
+        <v>50</v>
       </c>
       <c r="M20" t="n">
         <v>1.599185943603516</v>
@@ -1894,7 +1894,7 @@
         <v>1</v>
       </c>
       <c r="O20" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="P20" t="inlineStr">
         <is>
@@ -1958,7 +1958,7 @@
         <v>32</v>
       </c>
       <c r="L21" t="n">
-        <v>56.99999928474426</v>
+        <v>67.00000166893005</v>
       </c>
       <c r="M21" t="n">
         <v>1.599185943603516</v>
@@ -1967,7 +1967,7 @@
         <v>1</v>
       </c>
       <c r="O21" t="n">
-        <v>0.04</v>
+        <v>0.26</v>
       </c>
       <c r="P21" t="inlineStr">
         <is>
@@ -2104,7 +2104,7 @@
         <v>16</v>
       </c>
       <c r="L23" t="n">
-        <v>56.99999928474426</v>
+        <v>81.00000023841858</v>
       </c>
       <c r="M23" t="n">
         <v>1.599185943603516</v>
@@ -2113,7 +2113,7 @@
         <v>1</v>
       </c>
       <c r="O23" t="n">
-        <v>0.1</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="P23" t="inlineStr">
         <is>
@@ -2323,7 +2323,7 @@
         <v>16</v>
       </c>
       <c r="L26" t="n">
-        <v>89.99999761581421</v>
+        <v>92.00000166893005</v>
       </c>
       <c r="M26" t="n">
         <v>1.621250152587891</v>
@@ -2332,7 +2332,7 @@
         <v>1</v>
       </c>
       <c r="O26" t="n">
-        <v>0.86</v>
+        <v>0.82</v>
       </c>
       <c r="P26" t="inlineStr">
         <is>
@@ -2396,7 +2396,7 @@
         <v>32</v>
       </c>
       <c r="L27" t="n">
-        <v>69.9999988079071</v>
+        <v>56.00000023841858</v>
       </c>
       <c r="M27" t="n">
         <v>1.621250152587891</v>
@@ -2405,7 +2405,7 @@
         <v>1</v>
       </c>
       <c r="O27" t="n">
-        <v>0.38</v>
+        <v>0.1</v>
       </c>
       <c r="P27" t="inlineStr">
         <is>
@@ -2469,7 +2469,7 @@
         <v>64</v>
       </c>
       <c r="L28" t="n">
-        <v>60.00000238418579</v>
+        <v>50.99999904632568</v>
       </c>
       <c r="M28" t="n">
         <v>1.621250152587891</v>
@@ -2478,7 +2478,7 @@
         <v>1</v>
       </c>
       <c r="O28" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="P28" t="inlineStr">
         <is>
@@ -2542,16 +2542,16 @@
         <v>16</v>
       </c>
       <c r="L29" t="n">
-        <v>93.00000071525574</v>
+        <v>87.00000047683716</v>
       </c>
       <c r="M29" t="n">
         <v>1.621250152587891</v>
       </c>
       <c r="N29" t="n">
-        <v>0.92</v>
+        <v>0.96</v>
       </c>
       <c r="O29" t="n">
-        <v>0.96</v>
+        <v>0.78</v>
       </c>
       <c r="P29" t="inlineStr">
         <is>
@@ -2615,7 +2615,7 @@
         <v>32</v>
       </c>
       <c r="L30" t="n">
-        <v>67.00000166893005</v>
+        <v>55.0000011920929</v>
       </c>
       <c r="M30" t="n">
         <v>1.621250152587891</v>
@@ -2624,7 +2624,7 @@
         <v>1</v>
       </c>
       <c r="O30" t="n">
-        <v>0.3</v>
+        <v>0.06</v>
       </c>
       <c r="P30" t="inlineStr">
         <is>
@@ -2688,7 +2688,7 @@
         <v>64</v>
       </c>
       <c r="L31" t="n">
-        <v>62.00000047683716</v>
+        <v>62.99999952316284</v>
       </c>
       <c r="M31" t="n">
         <v>1.621250152587891</v>
@@ -2761,7 +2761,7 @@
         <v>16</v>
       </c>
       <c r="L32" t="n">
-        <v>72.00000286102295</v>
+        <v>70.99999785423279</v>
       </c>
       <c r="M32" t="n">
         <v>0.8241310119628906</v>
@@ -2770,7 +2770,7 @@
         <v>1</v>
       </c>
       <c r="O32" t="n">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="P32" t="inlineStr">
         <is>
@@ -2834,7 +2834,7 @@
         <v>32</v>
       </c>
       <c r="L33" t="n">
-        <v>56.99999928474426</v>
+        <v>52.99999713897705</v>
       </c>
       <c r="M33" t="n">
         <v>0.8241310119628906</v>
@@ -2843,7 +2843,7 @@
         <v>1</v>
       </c>
       <c r="O33" t="n">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="P33" t="inlineStr">
         <is>
@@ -2907,16 +2907,16 @@
         <v>64</v>
       </c>
       <c r="L34" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="M34" t="n">
         <v>0.8241310119628906</v>
       </c>
       <c r="N34" t="n">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="O34" t="n">
-        <v>0.32</v>
+        <v>0</v>
       </c>
       <c r="P34" t="inlineStr">
         <is>
@@ -2980,7 +2980,7 @@
         <v>16</v>
       </c>
       <c r="L35" t="n">
-        <v>54.00000214576721</v>
+        <v>76.99999809265137</v>
       </c>
       <c r="M35" t="n">
         <v>0.8241310119628906</v>
@@ -2989,7 +2989,7 @@
         <v>1</v>
       </c>
       <c r="O35" t="n">
-        <v>0.08</v>
+        <v>0.42</v>
       </c>
       <c r="P35" t="inlineStr">
         <is>
@@ -3053,7 +3053,7 @@
         <v>32</v>
       </c>
       <c r="L36" t="n">
-        <v>54.00000214576721</v>
+        <v>67.00000166893005</v>
       </c>
       <c r="M36" t="n">
         <v>0.8241310119628906</v>
@@ -3062,7 +3062,7 @@
         <v>1</v>
       </c>
       <c r="O36" t="n">
-        <v>0.08</v>
+        <v>0.3</v>
       </c>
       <c r="P36" t="inlineStr">
         <is>
@@ -3126,7 +3126,7 @@
         <v>64</v>
       </c>
       <c r="L37" t="n">
-        <v>50</v>
+        <v>62.00000047683716</v>
       </c>
       <c r="M37" t="n">
         <v>0.8241310119628906</v>
@@ -3135,7 +3135,7 @@
         <v>1</v>
       </c>
       <c r="O37" t="n">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="P37" t="inlineStr">
         <is>
@@ -3199,16 +3199,16 @@
         <v>16</v>
       </c>
       <c r="L38" t="n">
-        <v>97.00000286102295</v>
+        <v>88.99999856948853</v>
       </c>
       <c r="M38" t="n">
         <v>1.610507965087891</v>
       </c>
       <c r="N38" t="n">
-        <v>0.98</v>
+        <v>0.96</v>
       </c>
       <c r="O38" t="n">
-        <v>0.92</v>
+        <v>0.88</v>
       </c>
       <c r="P38" t="inlineStr">
         <is>
@@ -3272,16 +3272,16 @@
         <v>32</v>
       </c>
       <c r="L39" t="n">
-        <v>75</v>
+        <v>95.99999785423279</v>
       </c>
       <c r="M39" t="n">
         <v>1.610507965087891</v>
       </c>
       <c r="N39" t="n">
-        <v>0.66</v>
+        <v>0.98</v>
       </c>
       <c r="O39" t="n">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="P39" t="inlineStr">
         <is>
@@ -3345,16 +3345,16 @@
         <v>64</v>
       </c>
       <c r="L40" t="n">
-        <v>56.99999928474426</v>
+        <v>79.00000214576721</v>
       </c>
       <c r="M40" t="n">
         <v>1.610507965087891</v>
       </c>
       <c r="N40" t="n">
-        <v>1</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="O40" t="n">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="P40" t="inlineStr">
         <is>
@@ -3418,16 +3418,16 @@
         <v>16</v>
       </c>
       <c r="L41" t="n">
-        <v>93.99999976158142</v>
+        <v>82.99999833106995</v>
       </c>
       <c r="M41" t="n">
         <v>1.610507965087891</v>
       </c>
       <c r="N41" t="n">
-        <v>1</v>
+        <v>0.82</v>
       </c>
       <c r="O41" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="P41" t="inlineStr">
         <is>
@@ -3491,16 +3491,16 @@
         <v>32</v>
       </c>
       <c r="L42" t="n">
-        <v>77.99999713897705</v>
+        <v>80.0000011920929</v>
       </c>
       <c r="M42" t="n">
         <v>1.610507965087891</v>
       </c>
       <c r="N42" t="n">
-        <v>0.76</v>
+        <v>0.62</v>
       </c>
       <c r="O42" t="n">
-        <v>0.92</v>
+        <v>1</v>
       </c>
       <c r="P42" t="inlineStr">
         <is>
@@ -3564,16 +3564,16 @@
         <v>64</v>
       </c>
       <c r="L43" t="n">
-        <v>75.99999904632568</v>
+        <v>66.00000262260437</v>
       </c>
       <c r="M43" t="n">
         <v>1.610507965087891</v>
       </c>
       <c r="N43" t="n">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="O43" t="n">
-        <v>0.34</v>
+        <v>0.2</v>
       </c>
       <c r="P43" t="inlineStr">
         <is>
@@ -3637,7 +3637,7 @@
         <v>16</v>
       </c>
       <c r="L44" t="n">
-        <v>69.9999988079071</v>
+        <v>56.00000023841858</v>
       </c>
       <c r="M44" t="n">
         <v>0.8133888244628906</v>
@@ -3646,7 +3646,7 @@
         <v>1</v>
       </c>
       <c r="O44" t="n">
-        <v>0.26</v>
+        <v>0.08</v>
       </c>
       <c r="P44" t="inlineStr">
         <is>
@@ -3710,7 +3710,7 @@
         <v>32</v>
       </c>
       <c r="L45" t="n">
-        <v>56.99999928474426</v>
+        <v>58.99999737739563</v>
       </c>
       <c r="M45" t="n">
         <v>0.8133888244628906</v>
@@ -3719,7 +3719,7 @@
         <v>1</v>
       </c>
       <c r="O45" t="n">
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
       <c r="P45" t="inlineStr">
         <is>
@@ -3856,7 +3856,7 @@
         <v>16</v>
       </c>
       <c r="L47" t="n">
-        <v>76.99999809265137</v>
+        <v>73.00000190734863</v>
       </c>
       <c r="M47" t="n">
         <v>0.8133888244628906</v>
@@ -3865,7 +3865,7 @@
         <v>1</v>
       </c>
       <c r="O47" t="n">
-        <v>0.38</v>
+        <v>0.32</v>
       </c>
       <c r="P47" t="inlineStr">
         <is>
@@ -3929,7 +3929,7 @@
         <v>32</v>
       </c>
       <c r="L48" t="n">
-        <v>72.00000286102295</v>
+        <v>81.00000023841858</v>
       </c>
       <c r="M48" t="n">
         <v>0.8133888244628906</v>
@@ -3938,7 +3938,7 @@
         <v>1</v>
       </c>
       <c r="O48" t="n">
-        <v>0.36</v>
+        <v>0.58</v>
       </c>
       <c r="P48" t="inlineStr">
         <is>
@@ -4075,16 +4075,16 @@
         <v>16</v>
       </c>
       <c r="L50" t="n">
-        <v>81.99999928474426</v>
+        <v>91.00000262260437</v>
       </c>
       <c r="M50" t="n">
         <v>3.181461334228516</v>
       </c>
       <c r="N50" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="O50" t="n">
-        <v>0.6</v>
+        <v>0.84</v>
       </c>
       <c r="P50" t="inlineStr">
         <is>
@@ -4148,16 +4148,16 @@
         <v>32</v>
       </c>
       <c r="L51" t="n">
-        <v>81.99999928474426</v>
+        <v>63.99999856948853</v>
       </c>
       <c r="M51" t="n">
         <v>3.181461334228516</v>
       </c>
       <c r="N51" t="n">
-        <v>0.9399999999999999</v>
+        <v>1</v>
       </c>
       <c r="O51" t="n">
-        <v>0.66</v>
+        <v>0.24</v>
       </c>
       <c r="P51" t="inlineStr">
         <is>
@@ -4221,7 +4221,7 @@
         <v>64</v>
       </c>
       <c r="L52" t="n">
-        <v>50</v>
+        <v>51.99999809265137</v>
       </c>
       <c r="M52" t="n">
         <v>3.181461334228516</v>
@@ -4294,16 +4294,16 @@
         <v>16</v>
       </c>
       <c r="L53" t="n">
-        <v>94.9999988079071</v>
+        <v>87.99999952316284</v>
       </c>
       <c r="M53" t="n">
         <v>3.181461334228516</v>
       </c>
       <c r="N53" t="n">
-        <v>0.96</v>
+        <v>0.84</v>
       </c>
       <c r="O53" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="P53" t="inlineStr">
         <is>
@@ -4367,16 +4367,16 @@
         <v>32</v>
       </c>
       <c r="L54" t="n">
-        <v>87.00000047683716</v>
+        <v>55.0000011920929</v>
       </c>
       <c r="M54" t="n">
         <v>3.181461334228516</v>
       </c>
       <c r="N54" t="n">
-        <v>0.88</v>
+        <v>1</v>
       </c>
       <c r="O54" t="n">
-        <v>0.78</v>
+        <v>0.06</v>
       </c>
       <c r="P54" t="inlineStr">
         <is>
@@ -4440,7 +4440,7 @@
         <v>64</v>
       </c>
       <c r="L55" t="n">
-        <v>67.00000166893005</v>
+        <v>85.00000238418579</v>
       </c>
       <c r="M55" t="n">
         <v>3.181461334228516</v>
@@ -4449,7 +4449,7 @@
         <v>1</v>
       </c>
       <c r="O55" t="n">
-        <v>0.28</v>
+        <v>0.58</v>
       </c>
       <c r="P55" t="inlineStr">
         <is>
@@ -4513,16 +4513,16 @@
         <v>16</v>
       </c>
       <c r="L56" t="n">
-        <v>77.99999713897705</v>
+        <v>87.00000047683716</v>
       </c>
       <c r="M56" t="n">
         <v>1.603092193603516</v>
       </c>
       <c r="N56" t="n">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="O56" t="n">
-        <v>0.34</v>
+        <v>0.58</v>
       </c>
       <c r="P56" t="inlineStr">
         <is>
@@ -4586,16 +4586,16 @@
         <v>32</v>
       </c>
       <c r="L57" t="n">
-        <v>70.99999785423279</v>
+        <v>61.00000143051147</v>
       </c>
       <c r="M57" t="n">
         <v>1.603092193603516</v>
       </c>
       <c r="N57" t="n">
-        <v>0.9399999999999999</v>
+        <v>1</v>
       </c>
       <c r="O57" t="n">
-        <v>0.42</v>
+        <v>0.12</v>
       </c>
       <c r="P57" t="inlineStr">
         <is>
@@ -4659,7 +4659,7 @@
         <v>64</v>
       </c>
       <c r="L58" t="n">
-        <v>58.99999737739563</v>
+        <v>50</v>
       </c>
       <c r="M58" t="n">
         <v>1.603092193603516</v>
@@ -4668,7 +4668,7 @@
         <v>1</v>
       </c>
       <c r="O58" t="n">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="P58" t="inlineStr">
         <is>
@@ -4732,7 +4732,7 @@
         <v>16</v>
       </c>
       <c r="L59" t="n">
-        <v>61.00000143051147</v>
+        <v>63.99999856948853</v>
       </c>
       <c r="M59" t="n">
         <v>1.603092193603516</v>
@@ -4741,7 +4741,7 @@
         <v>1</v>
       </c>
       <c r="O59" t="n">
-        <v>0.14</v>
+        <v>0.2</v>
       </c>
       <c r="P59" t="inlineStr">
         <is>
@@ -4805,16 +4805,16 @@
         <v>32</v>
       </c>
       <c r="L60" t="n">
-        <v>63.99999856948853</v>
+        <v>69.9999988079071</v>
       </c>
       <c r="M60" t="n">
         <v>1.603092193603516</v>
       </c>
       <c r="N60" t="n">
-        <v>1</v>
+        <v>0.92</v>
       </c>
       <c r="O60" t="n">
-        <v>0.2</v>
+        <v>0.48</v>
       </c>
       <c r="P60" t="inlineStr">
         <is>
@@ -4878,7 +4878,7 @@
         <v>64</v>
       </c>
       <c r="L61" t="n">
-        <v>56.99999928474426</v>
+        <v>60.00000238418579</v>
       </c>
       <c r="M61" t="n">
         <v>1.603092193603516</v>
@@ -4887,7 +4887,7 @@
         <v>1</v>
       </c>
       <c r="O61" t="n">
-        <v>0.06</v>
+        <v>0.14</v>
       </c>
       <c r="P61" t="inlineStr">
         <is>
@@ -4951,16 +4951,16 @@
         <v>16</v>
       </c>
       <c r="L62" t="n">
-        <v>75</v>
+        <v>70.99999785423279</v>
       </c>
       <c r="M62" t="n">
         <v>3.172183990478516</v>
       </c>
       <c r="N62" t="n">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="O62" t="n">
-        <v>0.36</v>
+        <v>0.3</v>
       </c>
       <c r="P62" t="inlineStr">
         <is>
@@ -5024,16 +5024,16 @@
         <v>32</v>
       </c>
       <c r="L63" t="n">
-        <v>80.0000011920929</v>
+        <v>91.00000262260437</v>
       </c>
       <c r="M63" t="n">
         <v>3.172183990478516</v>
       </c>
       <c r="N63" t="n">
-        <v>1</v>
+        <v>0.92</v>
       </c>
       <c r="O63" t="n">
-        <v>0.42</v>
+        <v>0.86</v>
       </c>
       <c r="P63" t="inlineStr">
         <is>
@@ -5106,7 +5106,7 @@
         <v>1</v>
       </c>
       <c r="O64" t="n">
-        <v>0.28</v>
+        <v>0.22</v>
       </c>
       <c r="P64" t="inlineStr">
         <is>
@@ -5170,16 +5170,16 @@
         <v>16</v>
       </c>
       <c r="L65" t="n">
-        <v>93.99999976158142</v>
+        <v>74.00000095367432</v>
       </c>
       <c r="M65" t="n">
         <v>3.172183990478516</v>
       </c>
       <c r="N65" t="n">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="O65" t="n">
-        <v>0.82</v>
+        <v>0.4</v>
       </c>
       <c r="P65" t="inlineStr">
         <is>
@@ -5243,16 +5243,16 @@
         <v>32</v>
       </c>
       <c r="L66" t="n">
-        <v>88.99999856948853</v>
+        <v>87.00000047683716</v>
       </c>
       <c r="M66" t="n">
         <v>3.172183990478516</v>
       </c>
       <c r="N66" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="O66" t="n">
         <v>0.84</v>
-      </c>
-      <c r="O66" t="n">
-        <v>0.76</v>
       </c>
       <c r="P66" t="inlineStr">
         <is>
@@ -5316,7 +5316,7 @@
         <v>64</v>
       </c>
       <c r="L67" t="n">
-        <v>67.00000166893005</v>
+        <v>74.00000095367432</v>
       </c>
       <c r="M67" t="n">
         <v>3.172183990478516</v>
@@ -5325,7 +5325,7 @@
         <v>1</v>
       </c>
       <c r="O67" t="n">
-        <v>0.18</v>
+        <v>0.44</v>
       </c>
       <c r="P67" t="inlineStr">
         <is>
@@ -5389,7 +5389,7 @@
         <v>16</v>
       </c>
       <c r="L68" t="n">
-        <v>74.00000095367432</v>
+        <v>51.99999809265137</v>
       </c>
       <c r="M68" t="n">
         <v>1.593814849853516</v>
@@ -5398,7 +5398,7 @@
         <v>1</v>
       </c>
       <c r="O68" t="n">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="P68" t="inlineStr">
         <is>
@@ -5462,16 +5462,16 @@
         <v>32</v>
       </c>
       <c r="L69" t="n">
-        <v>76.99999809265137</v>
+        <v>86.00000143051147</v>
       </c>
       <c r="M69" t="n">
         <v>1.593814849853516</v>
       </c>
       <c r="N69" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="O69" t="n">
-        <v>0.38</v>
+        <v>0.66</v>
       </c>
       <c r="P69" t="inlineStr">
         <is>
@@ -5608,7 +5608,7 @@
         <v>16</v>
       </c>
       <c r="L71" t="n">
-        <v>68.00000071525574</v>
+        <v>73.00000190734863</v>
       </c>
       <c r="M71" t="n">
         <v>1.593814849853516</v>
@@ -5617,7 +5617,7 @@
         <v>1</v>
       </c>
       <c r="O71" t="n">
-        <v>0.2</v>
+        <v>0.34</v>
       </c>
       <c r="P71" t="inlineStr">
         <is>
@@ -5681,7 +5681,7 @@
         <v>32</v>
       </c>
       <c r="L72" t="n">
-        <v>89.99999761581421</v>
+        <v>68.99999976158142</v>
       </c>
       <c r="M72" t="n">
         <v>1.593814849853516</v>
@@ -5690,7 +5690,7 @@
         <v>1</v>
       </c>
       <c r="O72" t="n">
-        <v>0.64</v>
+        <v>0.28</v>
       </c>
       <c r="P72" t="inlineStr">
         <is>
@@ -5754,7 +5754,7 @@
         <v>64</v>
       </c>
       <c r="L73" t="n">
-        <v>51.99999809265137</v>
+        <v>50</v>
       </c>
       <c r="M73" t="n">
         <v>1.593814849853516</v>
@@ -5827,13 +5827,13 @@
         <v>16</v>
       </c>
       <c r="L74" t="n">
-        <v>81.00000023841858</v>
+        <v>82.99999833106995</v>
       </c>
       <c r="M74" t="n">
         <v>1.612705230712891</v>
       </c>
       <c r="N74" t="n">
-        <v>0.7</v>
+        <v>0.86</v>
       </c>
       <c r="O74" t="n">
         <v>1</v>
@@ -5900,13 +5900,13 @@
         <v>32</v>
       </c>
       <c r="L75" t="n">
-        <v>75</v>
+        <v>82.99999833106995</v>
       </c>
       <c r="M75" t="n">
         <v>1.612705230712891</v>
       </c>
       <c r="N75" t="n">
-        <v>0.62</v>
+        <v>0.76</v>
       </c>
       <c r="O75" t="n">
         <v>1</v>
@@ -5973,16 +5973,16 @@
         <v>64</v>
       </c>
       <c r="L76" t="n">
-        <v>88.99999856948853</v>
+        <v>81.99999928474426</v>
       </c>
       <c r="M76" t="n">
         <v>1.612705230712891</v>
       </c>
       <c r="N76" t="n">
-        <v>0.98</v>
+        <v>0.84</v>
       </c>
       <c r="O76" t="n">
-        <v>0.72</v>
+        <v>1</v>
       </c>
       <c r="P76" t="inlineStr">
         <is>
@@ -6046,16 +6046,16 @@
         <v>16</v>
       </c>
       <c r="L77" t="n">
-        <v>92.00000166893005</v>
+        <v>86.00000143051147</v>
       </c>
       <c r="M77" t="n">
         <v>1.612705230712891</v>
       </c>
       <c r="N77" t="n">
-        <v>0.98</v>
+        <v>0.9</v>
       </c>
       <c r="O77" t="n">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="P77" t="inlineStr">
         <is>
@@ -6119,16 +6119,16 @@
         <v>32</v>
       </c>
       <c r="L78" t="n">
-        <v>89.99999761581421</v>
+        <v>85.00000238418579</v>
       </c>
       <c r="M78" t="n">
         <v>1.612705230712891</v>
       </c>
       <c r="N78" t="n">
-        <v>0.9</v>
+        <v>0.76</v>
       </c>
       <c r="O78" t="n">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="P78" t="inlineStr">
         <is>
@@ -6192,7 +6192,7 @@
         <v>64</v>
       </c>
       <c r="L79" t="n">
-        <v>83.99999737739563</v>
+        <v>80.0000011920929</v>
       </c>
       <c r="M79" t="n">
         <v>1.612705230712891</v>
@@ -6201,7 +6201,7 @@
         <v>0.9399999999999999</v>
       </c>
       <c r="O79" t="n">
-        <v>0.62</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="P79" t="inlineStr">
         <is>
@@ -6265,7 +6265,7 @@
         <v>16</v>
       </c>
       <c r="L80" t="n">
-        <v>72.00000286102295</v>
+        <v>81.99999928474426</v>
       </c>
       <c r="M80" t="n">
         <v>0.8155860900878906</v>
@@ -6274,7 +6274,7 @@
         <v>0.96</v>
       </c>
       <c r="O80" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="P80" t="inlineStr">
         <is>
@@ -6338,7 +6338,7 @@
         <v>32</v>
       </c>
       <c r="L81" t="n">
-        <v>56.00000023841858</v>
+        <v>87.00000047683716</v>
       </c>
       <c r="M81" t="n">
         <v>0.8155860900878906</v>
@@ -6347,7 +6347,7 @@
         <v>1</v>
       </c>
       <c r="O81" t="n">
-        <v>0.08</v>
+        <v>0.66</v>
       </c>
       <c r="P81" t="inlineStr">
         <is>
@@ -6411,7 +6411,7 @@
         <v>64</v>
       </c>
       <c r="L82" t="n">
-        <v>74.00000095367432</v>
+        <v>50</v>
       </c>
       <c r="M82" t="n">
         <v>0.8155860900878906</v>
@@ -6420,7 +6420,7 @@
         <v>1</v>
       </c>
       <c r="O82" t="n">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="P82" t="inlineStr">
         <is>
@@ -6484,7 +6484,7 @@
         <v>16</v>
       </c>
       <c r="L83" t="n">
-        <v>74.00000095367432</v>
+        <v>61.00000143051147</v>
       </c>
       <c r="M83" t="n">
         <v>0.8155860900878906</v>
@@ -6493,7 +6493,7 @@
         <v>1</v>
       </c>
       <c r="O83" t="n">
-        <v>0.36</v>
+        <v>0.14</v>
       </c>
       <c r="P83" t="inlineStr">
         <is>
@@ -6557,7 +6557,7 @@
         <v>32</v>
       </c>
       <c r="L84" t="n">
-        <v>52.99999713897705</v>
+        <v>68.99999976158142</v>
       </c>
       <c r="M84" t="n">
         <v>0.8155860900878906</v>
@@ -6566,7 +6566,7 @@
         <v>1</v>
       </c>
       <c r="O84" t="n">
-        <v>0.06</v>
+        <v>0.32</v>
       </c>
       <c r="P84" t="inlineStr">
         <is>
@@ -6630,7 +6630,7 @@
         <v>64</v>
       </c>
       <c r="L85" t="n">
-        <v>66.00000262260437</v>
+        <v>52.99999713897705</v>
       </c>
       <c r="M85" t="n">
         <v>0.8155860900878906</v>
@@ -6639,7 +6639,7 @@
         <v>1</v>
       </c>
       <c r="O85" t="n">
-        <v>0.18</v>
+        <v>0.04</v>
       </c>
       <c r="P85" t="inlineStr">
         <is>
@@ -6703,16 +6703,16 @@
         <v>16</v>
       </c>
       <c r="L86" t="n">
-        <v>86.00000143051147</v>
+        <v>94.9999988079071</v>
       </c>
       <c r="M86" t="n">
         <v>1.607334136962891</v>
       </c>
       <c r="N86" t="n">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="O86" t="n">
-        <v>0.54</v>
+        <v>1</v>
       </c>
       <c r="P86" t="inlineStr">
         <is>
@@ -6776,7 +6776,7 @@
         <v>32</v>
       </c>
       <c r="L87" t="n">
-        <v>72.00000286102295</v>
+        <v>61.00000143051147</v>
       </c>
       <c r="M87" t="n">
         <v>1.607334136962891</v>
@@ -6785,7 +6785,7 @@
         <v>1</v>
       </c>
       <c r="O87" t="n">
-        <v>0.38</v>
+        <v>0.18</v>
       </c>
       <c r="P87" t="inlineStr">
         <is>
@@ -6849,7 +6849,7 @@
         <v>64</v>
       </c>
       <c r="L88" t="n">
-        <v>50.99999904632568</v>
+        <v>56.99999928474426</v>
       </c>
       <c r="M88" t="n">
         <v>1.607334136962891</v>
@@ -6858,7 +6858,7 @@
         <v>1</v>
       </c>
       <c r="O88" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="P88" t="inlineStr">
         <is>
@@ -6922,16 +6922,16 @@
         <v>16</v>
       </c>
       <c r="L89" t="n">
-        <v>91.00000262260437</v>
+        <v>81.99999928474426</v>
       </c>
       <c r="M89" t="n">
         <v>1.607334136962891</v>
       </c>
       <c r="N89" t="n">
-        <v>0.9399999999999999</v>
+        <v>1</v>
       </c>
       <c r="O89" t="n">
-        <v>0.74</v>
+        <v>0.5</v>
       </c>
       <c r="P89" t="inlineStr">
         <is>
@@ -6995,7 +6995,7 @@
         <v>32</v>
       </c>
       <c r="L90" t="n">
-        <v>75</v>
+        <v>83.99999737739563</v>
       </c>
       <c r="M90" t="n">
         <v>1.607334136962891</v>
@@ -7004,7 +7004,7 @@
         <v>1</v>
       </c>
       <c r="O90" t="n">
-        <v>0.4</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="P90" t="inlineStr">
         <is>
@@ -7068,7 +7068,7 @@
         <v>64</v>
       </c>
       <c r="L91" t="n">
-        <v>67.00000166893005</v>
+        <v>95.99999785423279</v>
       </c>
       <c r="M91" t="n">
         <v>1.607334136962891</v>
@@ -7077,7 +7077,7 @@
         <v>1</v>
       </c>
       <c r="O91" t="n">
-        <v>0.28</v>
+        <v>0.88</v>
       </c>
       <c r="P91" t="inlineStr">
         <is>
@@ -7141,7 +7141,7 @@
         <v>16</v>
       </c>
       <c r="L92" t="n">
-        <v>75</v>
+        <v>61.00000143051147</v>
       </c>
       <c r="M92" t="n">
         <v>0.8102149963378906</v>
@@ -7150,7 +7150,7 @@
         <v>1</v>
       </c>
       <c r="O92" t="n">
-        <v>0.34</v>
+        <v>0.14</v>
       </c>
       <c r="P92" t="inlineStr">
         <is>
@@ -7214,7 +7214,7 @@
         <v>32</v>
       </c>
       <c r="L93" t="n">
-        <v>55.0000011920929</v>
+        <v>54.00000214576721</v>
       </c>
       <c r="M93" t="n">
         <v>0.8102149963378906</v>
@@ -7223,7 +7223,7 @@
         <v>1</v>
       </c>
       <c r="O93" t="n">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="P93" t="inlineStr">
         <is>
@@ -7360,7 +7360,7 @@
         <v>16</v>
       </c>
       <c r="L95" t="n">
-        <v>76.99999809265137</v>
+        <v>69.9999988079071</v>
       </c>
       <c r="M95" t="n">
         <v>0.8102149963378906</v>
@@ -7369,7 +7369,7 @@
         <v>1</v>
       </c>
       <c r="O95" t="n">
-        <v>0.42</v>
+        <v>0.34</v>
       </c>
       <c r="P95" t="inlineStr">
         <is>
@@ -7433,7 +7433,7 @@
         <v>32</v>
       </c>
       <c r="L96" t="n">
-        <v>69.9999988079071</v>
+        <v>61.00000143051147</v>
       </c>
       <c r="M96" t="n">
         <v>0.8102149963378906</v>
@@ -7442,7 +7442,7 @@
         <v>1</v>
       </c>
       <c r="O96" t="n">
-        <v>0.34</v>
+        <v>0.16</v>
       </c>
       <c r="P96" t="inlineStr">
         <is>
@@ -7506,7 +7506,7 @@
         <v>64</v>
       </c>
       <c r="L97" t="n">
-        <v>55.0000011920929</v>
+        <v>50</v>
       </c>
       <c r="M97" t="n">
         <v>0.8102149963378906</v>
@@ -7515,7 +7515,7 @@
         <v>1</v>
       </c>
       <c r="O97" t="n">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="P97" t="inlineStr">
         <is>

</xml_diff>